<commit_message>
June20 2025 Added Files in the NinjaV9 repository
</commit_message>
<xml_diff>
--- a/testData/NinjaDataSheet.xlsx
+++ b/testData/NinjaDataSheet.xlsx
@@ -40,28 +40,28 @@
     <t xml:space="preserve">test@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">test121@test.com</t>
+    <t xml:space="preserve">sid@cloudberry.services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otisdog22@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234QWERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shalaka.dongre@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testselenium12345@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">test123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sid@cloudberry.services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otisdog22@yahoo.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234QWERT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shalaka.dongre@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test123!</t>
   </si>
 </sst>
 </file>
@@ -256,10 +256,10 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.18"/>
@@ -289,7 +289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -297,7 +297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -305,7 +305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -313,17 +313,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="ma12345678@gmail.com"/>
+    <hyperlink ref="A7" r:id="rId2" display="testselenium12345@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
June20 2025 Updated Files
</commit_message>
<xml_diff>
--- a/testData/NinjaDataSheet.xlsx
+++ b/testData/NinjaDataSheet.xlsx
@@ -40,28 +40,28 @@
     <t xml:space="preserve">test@1234</t>
   </si>
   <si>
-    <t xml:space="preserve">test121@test.com</t>
+    <t xml:space="preserve">sid@cloudberry.services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">otisdog22@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234QWERT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shalaka.dongre@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test123!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testselenium12345@gmail.com</t>
   </si>
   <si>
     <t xml:space="preserve">test123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sid@cloudberry.services</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test123</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otisdog22@yahoo.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1234QWERT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shalaka.dongre@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test123!</t>
   </si>
 </sst>
 </file>
@@ -256,10 +256,10 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.18"/>
@@ -289,7 +289,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -297,7 +297,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -305,7 +305,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -313,17 +313,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="ma12345678@gmail.com"/>
+    <hyperlink ref="A7" r:id="rId2" display="testselenium12345@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>